<commit_message>
Colmillo and Gavi geomorphology update
</commit_message>
<xml_diff>
--- a/Geomorphology/Comillo/Colmillo_notes.xlsx
+++ b/Geomorphology/Comillo/Colmillo_notes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://adminliveunc-my.sharepoint.com/personal/kriddie_ad_unc_edu/Documents/Ecuador2021/Ecuador2021/Geomorphology/Comillo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\whitm\OneDrive - University of North Carolina at Chapel Hill\Ecuador2021\Ecuador2021\Geomorphology\Comillo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="718" documentId="8_{8C76BE55-0E2E-44DA-8A4E-7FE7551E922B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B70EBAEF-B2B4-4B61-BCB2-8BA950B4D52E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39B9CC17-FF5D-47C8-A46A-E4297961AF24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{AD3F54C6-967E-4943-8224-5776EC6F2391}"/>
+    <workbookView xWindow="180" yWindow="320" windowWidth="14670" windowHeight="8580" xr2:uid="{AD3F54C6-967E-4943-8224-5776EC6F2391}"/>
   </bookViews>
   <sheets>
     <sheet name="July9 2021" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="137">
   <si>
     <t>Colmillo</t>
   </si>
@@ -244,12 +244,6 @@
     <t>Station 6</t>
   </si>
   <si>
-    <t>wypt 076</t>
-  </si>
-  <si>
-    <t>wypt 077</t>
-  </si>
-  <si>
     <t>syn 1</t>
   </si>
   <si>
@@ -320,6 +314,138 @@
   </si>
   <si>
     <t>Time</t>
+  </si>
+  <si>
+    <t>2021-07-16T14:45:46Z</t>
+  </si>
+  <si>
+    <t>2021-07-16T15:13:49Z</t>
+  </si>
+  <si>
+    <t>2021-07-16T15:14:52Z</t>
+  </si>
+  <si>
+    <t>2021-07-16T15:27:11Z</t>
+  </si>
+  <si>
+    <t>2021-07-16T15:30:31Z</t>
+  </si>
+  <si>
+    <t>2021-07-16T15:50:17Z</t>
+  </si>
+  <si>
+    <t>2021-07-16T15:49:17Z</t>
+  </si>
+  <si>
+    <t>2021-07-16T16:06:16Z</t>
+  </si>
+  <si>
+    <t>2021-07-16T16:11:14Z</t>
+  </si>
+  <si>
+    <t>2021-07-16T16:23:45Z</t>
+  </si>
+  <si>
+    <t>2021-07-16T16:25:48Z</t>
+  </si>
+  <si>
+    <t>2021-07-16T16:33:04Z</t>
+  </si>
+  <si>
+    <t>2021-07-16T16:43:19Z</t>
+  </si>
+  <si>
+    <t>2021-07-16T16:49:08Z</t>
+  </si>
+  <si>
+    <t>2021-07-16T16:55:28Z</t>
+  </si>
+  <si>
+    <t>2021-07-16T16:57:51Z</t>
+  </si>
+  <si>
+    <t>2021-07-16T17:12:17Z</t>
+  </si>
+  <si>
+    <t>2021-07-16T17:18:20Z</t>
+  </si>
+  <si>
+    <t>2021-07-16T17:42:13Z</t>
+  </si>
+  <si>
+    <t>2021-07-16T17:44:24Z</t>
+  </si>
+  <si>
+    <t>2021-07-16T17:48:06Z</t>
+  </si>
+  <si>
+    <t>2021-07-16T18:13:11Z</t>
+  </si>
+  <si>
+    <t>2021-07-16T18:39:42Z</t>
+  </si>
+  <si>
+    <t>2021-07-16T18:44:49Z</t>
+  </si>
+  <si>
+    <t>2021-07-16T18:48:57Z</t>
+  </si>
+  <si>
+    <t>2021-07-16T18:49:17Z</t>
+  </si>
+  <si>
+    <t>DateTIme</t>
+  </si>
+  <si>
+    <t>2021-07-09T16:29:03Z</t>
+  </si>
+  <si>
+    <t>2021-07-09T16:41:03Z</t>
+  </si>
+  <si>
+    <t>2021-07-09T16:48:30Z</t>
+  </si>
+  <si>
+    <t>2021-07-09T17:04:47Z</t>
+  </si>
+  <si>
+    <t>2021-07-09T17:17:47Z</t>
+  </si>
+  <si>
+    <t>2021-07-09T17:37:17Z</t>
+  </si>
+  <si>
+    <t>2021-07-09T17:50:23Z</t>
+  </si>
+  <si>
+    <t>2021-07-09T18:25:31Z</t>
+  </si>
+  <si>
+    <t>2021-07-09T18:29:37Z</t>
+  </si>
+  <si>
+    <t>2021-07-09T18:44:13Z</t>
+  </si>
+  <si>
+    <t>2021-07-09T18:56:24Z</t>
+  </si>
+  <si>
+    <t>2021-07-09T19:06:35Z</t>
+  </si>
+  <si>
+    <t>2021-07-09T19:44:34Z</t>
+  </si>
+  <si>
+    <t>2021-07-09T19:39:28Z</t>
+  </si>
+  <si>
+    <t>2021-07-09T19:51:45Z</t>
+  </si>
+  <si>
+    <t>2021-07-09T20:09:11Z</t>
+  </si>
+  <si>
+    <t>2021-07-09T20:24:37Z</t>
   </si>
 </sst>
 </file>
@@ -681,28 +807,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0766A555-290B-4D70-A6A9-9F46A6F8DC20}">
-  <dimension ref="A1:H104"/>
+  <dimension ref="A1:I104"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="K104" sqref="K104"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="G99" sqref="G99"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>44386</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -716,7 +843,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -730,7 +857,7 @@
         <v>3951.2114259999898</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -741,7 +868,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -763,8 +890,11 @@
       <c r="H10" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>0</v>
       </c>
@@ -789,8 +919,11 @@
       <c r="H11">
         <v>3951.2114259999898</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>10</v>
       </c>
@@ -801,7 +934,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>20</v>
       </c>
@@ -812,7 +945,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>30</v>
       </c>
@@ -823,7 +956,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>40</v>
       </c>
@@ -834,7 +967,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>42</v>
       </c>
@@ -859,8 +992,11 @@
       <c r="H16">
         <v>3947.2238769999899</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>50</v>
       </c>
@@ -871,7 +1007,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>60</v>
       </c>
@@ -882,7 +1018,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>70</v>
       </c>
@@ -893,7 +1029,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>80</v>
       </c>
@@ -904,7 +1040,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>90</v>
       </c>
@@ -915,7 +1051,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>93</v>
       </c>
@@ -940,8 +1076,11 @@
       <c r="H22">
         <v>3944.155029</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I22" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>100</v>
       </c>
@@ -952,7 +1091,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>110</v>
       </c>
@@ -963,7 +1102,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>120</v>
       </c>
@@ -974,7 +1113,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>130</v>
       </c>
@@ -985,7 +1124,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>139</v>
       </c>
@@ -999,7 +1138,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>140</v>
       </c>
@@ -1010,7 +1149,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>149</v>
       </c>
@@ -1024,7 +1163,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>150</v>
       </c>
@@ -1046,8 +1185,11 @@
       <c r="H30">
         <v>3941.26001</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I30" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>160</v>
       </c>
@@ -1058,7 +1200,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>170</v>
       </c>
@@ -1069,7 +1211,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>180</v>
       </c>
@@ -1080,7 +1222,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>182</v>
       </c>
@@ -1094,7 +1236,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>190</v>
       </c>
@@ -1105,7 +1247,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>194</v>
       </c>
@@ -1119,7 +1261,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>200</v>
       </c>
@@ -1141,8 +1283,11 @@
       <c r="H37">
         <v>3934.1328119999898</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I37" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>210</v>
       </c>
@@ -1153,7 +1298,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>216</v>
       </c>
@@ -1167,7 +1312,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>220</v>
       </c>
@@ -1178,7 +1323,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>230</v>
       </c>
@@ -1189,7 +1334,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>240</v>
       </c>
@@ -1200,7 +1345,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>250</v>
       </c>
@@ -1222,8 +1367,11 @@
       <c r="H43">
         <v>3932.3935550000001</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I43" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>260</v>
       </c>
@@ -1234,7 +1382,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>263</v>
       </c>
@@ -1248,7 +1396,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>270</v>
       </c>
@@ -1262,7 +1410,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>280</v>
       </c>
@@ -1273,7 +1421,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>286</v>
       </c>
@@ -1287,7 +1435,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>290</v>
       </c>
@@ -1298,7 +1446,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>300</v>
       </c>
@@ -1323,8 +1471,11 @@
       <c r="H50">
         <v>3933.9929200000001</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I50" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>301</v>
       </c>
@@ -1338,7 +1489,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>310</v>
       </c>
@@ -1349,7 +1500,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>320</v>
       </c>
@@ -1360,7 +1511,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>330</v>
       </c>
@@ -1371,7 +1522,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>338</v>
       </c>
@@ -1385,7 +1536,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>340</v>
       </c>
@@ -1396,7 +1547,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>350</v>
       </c>
@@ -1421,8 +1572,11 @@
       <c r="H57">
         <v>3927.8188479999899</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I57" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>360</v>
       </c>
@@ -1433,7 +1587,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>361</v>
       </c>
@@ -1447,7 +1601,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>370</v>
       </c>
@@ -1458,7 +1612,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>380</v>
       </c>
@@ -1469,7 +1623,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>390</v>
       </c>
@@ -1480,7 +1634,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>396</v>
       </c>
@@ -1494,7 +1648,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>400</v>
       </c>
@@ -1516,8 +1670,11 @@
       <c r="H64">
         <v>3927.303711</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I64" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>407</v>
       </c>
@@ -1531,7 +1688,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>410</v>
       </c>
@@ -1542,7 +1699,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>420</v>
       </c>
@@ -1553,7 +1710,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>430</v>
       </c>
@@ -1564,7 +1721,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>440</v>
       </c>
@@ -1575,7 +1732,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>445</v>
       </c>
@@ -1589,7 +1746,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>450</v>
       </c>
@@ -1611,8 +1768,11 @@
       <c r="H71">
         <v>3931.7722170000002</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I71" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>460</v>
       </c>
@@ -1623,7 +1783,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>470</v>
       </c>
@@ -1634,7 +1794,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>480</v>
       </c>
@@ -1648,7 +1808,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>490</v>
       </c>
@@ -1659,7 +1819,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>500</v>
       </c>
@@ -1684,8 +1844,11 @@
       <c r="H76">
         <v>3925.8413089999899</v>
       </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I76" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>510</v>
       </c>
@@ -1696,7 +1859,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>520</v>
       </c>
@@ -1707,7 +1870,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>530</v>
       </c>
@@ -1718,7 +1881,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>540</v>
       </c>
@@ -1729,7 +1892,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>550</v>
       </c>
@@ -1751,8 +1914,11 @@
       <c r="H81">
         <v>3924.3862300000001</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I81" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>560</v>
       </c>
@@ -1763,7 +1929,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>570</v>
       </c>
@@ -1774,7 +1940,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>580</v>
       </c>
@@ -1785,7 +1951,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>590</v>
       </c>
@@ -1799,7 +1965,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>600</v>
       </c>
@@ -1821,8 +1987,11 @@
       <c r="H86">
         <v>3924.6608890000002</v>
       </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I86" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>610</v>
       </c>
@@ -1833,7 +2002,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>620</v>
       </c>
@@ -1844,7 +2013,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>625</v>
       </c>
@@ -1858,7 +2027,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>630</v>
       </c>
@@ -1872,7 +2041,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>640</v>
       </c>
@@ -1883,7 +2052,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>650</v>
       </c>
@@ -1908,8 +2077,11 @@
       <c r="H92">
         <v>3924.4809570000002</v>
       </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I92" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>660</v>
       </c>
@@ -1923,7 +2095,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>670</v>
       </c>
@@ -1937,7 +2109,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>674</v>
       </c>
@@ -1951,7 +2123,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>680</v>
       </c>
@@ -1962,7 +2134,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>690</v>
       </c>
@@ -1973,7 +2145,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>700</v>
       </c>
@@ -1995,8 +2167,11 @@
       <c r="H98">
         <v>3921.5214839999899</v>
       </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I98" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>710</v>
       </c>
@@ -2021,8 +2196,11 @@
       <c r="H99">
         <v>3922.391357</v>
       </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I99" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>720</v>
       </c>
@@ -2033,7 +2211,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>730</v>
       </c>
@@ -2044,7 +2222,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>740</v>
       </c>
@@ -2055,7 +2233,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A103">
         <v>745</v>
       </c>
@@ -2069,7 +2247,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A104">
         <v>750</v>
       </c>
@@ -2090,6 +2268,9 @@
       </c>
       <c r="H104">
         <v>3922.8166500000002</v>
+      </c>
+      <c r="I104" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -2100,28 +2281,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25757DB2-562B-42A3-9BA7-006D7693D831}">
-  <dimension ref="A1:H94"/>
+  <dimension ref="A1:I94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N93" sqref="N93"/>
+    <sheetView topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="I93" sqref="I93:I94"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="1" max="1" width="18.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>44393</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>62</v>
       </c>
@@ -2129,7 +2310,7 @@
         <v>0.40625</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>61</v>
       </c>
@@ -2143,12 +2324,12 @@
         <v>43</v>
       </c>
       <c r="E5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B6">
         <v>-0.34898799844086198</v>
@@ -2163,14 +2344,14 @@
         <v>0.40625</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D8">
         <v>3921</v>
@@ -2179,7 +2360,7 @@
         <v>0.5756944444444444</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -2193,7 +2374,7 @@
         <v>8</v>
       </c>
       <c r="E11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F11" t="s">
         <v>41</v>
@@ -2205,7 +2386,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>0</v>
       </c>
@@ -2218,8 +2399,20 @@
       <c r="D12" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <v>-0.34898799844086198</v>
+      </c>
+      <c r="F12">
+        <v>-78.199237966910005</v>
+      </c>
+      <c r="G12">
+        <v>3895.2597660000001</v>
+      </c>
+      <c r="H12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13">
         <f>A12+10</f>
         <v>10</v>
@@ -2231,7 +2424,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14">
         <f t="shared" ref="A14:A80" si="0">A13+10</f>
         <v>20</v>
@@ -2243,7 +2436,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -2255,7 +2448,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -2267,7 +2460,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>45</v>
       </c>
@@ -2281,7 +2474,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>48</v>
       </c>
@@ -2294,20 +2487,20 @@
       <c r="D18" t="s">
         <v>68</v>
       </c>
-      <c r="E18" t="s">
-        <v>69</v>
+      <c r="E18">
+        <v>-0.34863403066992799</v>
       </c>
       <c r="F18">
-        <v>-0.34863403066992799</v>
+        <v>-78.199402000755001</v>
       </c>
       <c r="G18">
-        <v>-78.199402000755001</v>
-      </c>
-      <c r="H18">
         <v>3897.0820309999899</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H18" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19">
         <f>A16+10</f>
         <v>50</v>
@@ -2318,20 +2511,20 @@
       <c r="C19">
         <v>52</v>
       </c>
-      <c r="E19" t="s">
-        <v>70</v>
+      <c r="E19">
+        <v>-0.34862900152802501</v>
       </c>
       <c r="F19">
-        <v>-0.34862900152802501</v>
+        <v>-78.199443994089904</v>
       </c>
       <c r="G19">
-        <v>-78.199443994089904</v>
-      </c>
-      <c r="H19">
         <v>3892.4650879999899</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H19" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>60</v>
@@ -2343,7 +2536,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>70</v>
@@ -2355,7 +2548,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>80</v>
@@ -2367,7 +2560,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>83</v>
       </c>
@@ -2378,7 +2571,7 @@
         <v>25</v>
       </c>
       <c r="D23" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E23">
         <v>78</v>
@@ -2392,8 +2585,11 @@
       <c r="H23">
         <v>3903.203125</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I23" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24">
         <f>A22+10</f>
         <v>90</v>
@@ -2405,7 +2601,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -2417,7 +2613,7 @@
         <v>30</v>
       </c>
       <c r="D25" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E25">
         <v>79</v>
@@ -2431,8 +2627,11 @@
       <c r="H25">
         <v>3898.998779</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I25" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>110</v>
@@ -2444,7 +2643,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>120</v>
@@ -2456,7 +2655,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>130</v>
@@ -2468,7 +2667,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>134</v>
       </c>
@@ -2479,10 +2678,10 @@
         <v>10</v>
       </c>
       <c r="D29" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30">
         <f>A28+10</f>
         <v>140</v>
@@ -2494,7 +2693,7 @@
         <v>17</v>
       </c>
       <c r="D30" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E30">
         <v>83</v>
@@ -2508,8 +2707,11 @@
       <c r="H30">
         <v>3896.1145019999899</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I30" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>150</v>
@@ -2532,8 +2734,11 @@
       <c r="H31">
         <v>3896.844971</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I31" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>160</v>
@@ -2545,7 +2750,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>170</v>
@@ -2557,7 +2762,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34">
         <f t="shared" si="0"/>
         <v>180</v>
@@ -2569,7 +2774,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35">
         <f t="shared" si="0"/>
         <v>190</v>
@@ -2581,7 +2786,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>194</v>
       </c>
@@ -2606,8 +2811,11 @@
       <c r="H36">
         <v>3897.4208979999898</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I36" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37">
         <f>A35+10</f>
         <v>200</v>
@@ -2630,8 +2838,11 @@
       <c r="H37">
         <v>3897.7985840000001</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I37" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>202</v>
       </c>
@@ -2642,10 +2853,10 @@
         <v>10</v>
       </c>
       <c r="D38" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39">
         <f>A37+10</f>
         <v>210</v>
@@ -2657,7 +2868,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40">
         <f t="shared" si="0"/>
         <v>220</v>
@@ -2669,7 +2880,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41">
         <f t="shared" si="0"/>
         <v>230</v>
@@ -2681,7 +2892,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42">
         <f t="shared" si="0"/>
         <v>240</v>
@@ -2693,7 +2904,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>241</v>
       </c>
@@ -2704,7 +2915,7 @@
         <v>18</v>
       </c>
       <c r="D43" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E43">
         <v>86</v>
@@ -2718,8 +2929,11 @@
       <c r="H43">
         <v>3896.9291990000002</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I43" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>245</v>
       </c>
@@ -2730,10 +2944,10 @@
         <v>10</v>
       </c>
       <c r="D44" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>246</v>
       </c>
@@ -2744,10 +2958,10 @@
         <v>10</v>
       </c>
       <c r="D45" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46">
         <f>A42+10</f>
         <v>250</v>
@@ -2770,8 +2984,11 @@
       <c r="H46">
         <v>3899.2426759999898</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I46" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>258</v>
       </c>
@@ -2796,8 +3013,11 @@
       <c r="H47">
         <v>3901.7189939999898</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I47" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48">
         <f>A46+10</f>
         <v>260</v>
@@ -2809,7 +3029,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>261</v>
       </c>
@@ -2820,10 +3040,10 @@
         <v>10</v>
       </c>
       <c r="D49" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50">
         <f>A48+10</f>
         <v>270</v>
@@ -2835,7 +3055,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51">
         <f t="shared" si="0"/>
         <v>280</v>
@@ -2847,7 +3067,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52">
         <f t="shared" si="0"/>
         <v>290</v>
@@ -2859,7 +3079,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53">
         <f t="shared" si="0"/>
         <v>300</v>
@@ -2882,8 +3102,11 @@
       <c r="H53">
         <v>3897.3588869999899</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I53" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>305</v>
       </c>
@@ -2905,8 +3128,11 @@
       <c r="H54">
         <v>3899.016357</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I54" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>310</v>
       </c>
@@ -2917,7 +3143,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>320</v>
       </c>
@@ -2928,7 +3154,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>329</v>
       </c>
@@ -2942,7 +3168,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58">
         <f>A56+10</f>
         <v>330</v>
@@ -2954,7 +3180,7 @@
         <v>85</v>
       </c>
       <c r="D58" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E58">
         <v>91</v>
@@ -2968,8 +3194,11 @@
       <c r="H58">
         <v>3900.1557619999899</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I58" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59">
         <f t="shared" si="0"/>
         <v>340</v>
@@ -2981,10 +3210,10 @@
         <v>10</v>
       </c>
       <c r="D59" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>349</v>
       </c>
@@ -2995,10 +3224,10 @@
         <v>10</v>
       </c>
       <c r="D60" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61">
         <f>A59+10</f>
         <v>350</v>
@@ -3024,8 +3253,11 @@
       <c r="H61">
         <v>3902.286865</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I61" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62">
         <f t="shared" si="0"/>
         <v>360</v>
@@ -3037,10 +3269,10 @@
         <v>24</v>
       </c>
       <c r="D62" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63">
         <f t="shared" si="0"/>
         <v>370</v>
@@ -3052,7 +3284,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64">
         <f t="shared" si="0"/>
         <v>380</v>
@@ -3064,7 +3296,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>384</v>
       </c>
@@ -3089,8 +3321,11 @@
       <c r="H65">
         <v>3898.0927729999898</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I65" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>388</v>
       </c>
@@ -3101,10 +3336,10 @@
         <v>10</v>
       </c>
       <c r="D66" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A67">
         <f>A64+10</f>
         <v>390</v>
@@ -3116,7 +3351,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A68">
         <f t="shared" si="0"/>
         <v>400</v>
@@ -3139,8 +3374,11 @@
       <c r="H68">
         <v>3901.1948240000002</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I68" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A69">
         <f t="shared" si="0"/>
         <v>410</v>
@@ -3152,7 +3390,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A70">
         <f t="shared" si="0"/>
         <v>420</v>
@@ -3164,7 +3402,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>429</v>
       </c>
@@ -3189,8 +3427,11 @@
       <c r="H71">
         <v>3899.2807619999899</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I71" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A72">
         <f>A70+10</f>
         <v>430</v>
@@ -3213,8 +3454,11 @@
       <c r="H72">
         <v>3903.9938959999899</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I72" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>435</v>
       </c>
@@ -3225,10 +3469,10 @@
         <v>10</v>
       </c>
       <c r="D73" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A74">
         <f>A72+10</f>
         <v>440</v>
@@ -3240,10 +3484,10 @@
         <v>35</v>
       </c>
       <c r="D74" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>448</v>
       </c>
@@ -3254,10 +3498,10 @@
         <v>10</v>
       </c>
       <c r="D75" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A76">
         <f>A74+10</f>
         <v>450</v>
@@ -3280,8 +3524,11 @@
       <c r="H76">
         <v>3912.5498050000001</v>
       </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I76" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A77">
         <f t="shared" si="0"/>
         <v>460</v>
@@ -3293,7 +3540,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>467</v>
       </c>
@@ -3304,10 +3551,10 @@
         <v>10</v>
       </c>
       <c r="D78" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A79">
         <f>A77+10</f>
         <v>470</v>
@@ -3319,7 +3566,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A80">
         <f t="shared" si="0"/>
         <v>480</v>
@@ -3331,7 +3578,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A81">
         <f t="shared" ref="A81:A89" si="1">A80+10</f>
         <v>490</v>
@@ -3343,7 +3590,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A82">
         <f t="shared" si="1"/>
         <v>500</v>
@@ -3366,8 +3613,11 @@
       <c r="H82">
         <v>3915.4628910000001</v>
       </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I82" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A83">
         <f t="shared" si="1"/>
         <v>510</v>
@@ -3379,7 +3629,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A84">
         <f t="shared" si="1"/>
         <v>520</v>
@@ -3391,7 +3641,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A85">
         <f t="shared" si="1"/>
         <v>530</v>
@@ -3403,7 +3653,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A86">
         <f t="shared" si="1"/>
         <v>540</v>
@@ -3415,7 +3665,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A87">
         <f t="shared" si="1"/>
         <v>550</v>
@@ -3438,8 +3688,11 @@
       <c r="H87">
         <v>3922.6518550000001</v>
       </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I87" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A88">
         <f t="shared" si="1"/>
         <v>560</v>
@@ -3451,7 +3704,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A89">
         <f t="shared" si="1"/>
         <v>570</v>
@@ -3463,7 +3716,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>579</v>
       </c>
@@ -3474,7 +3727,7 @@
         <v>10</v>
       </c>
       <c r="D90" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E90">
         <v>102</v>
@@ -3488,8 +3741,11 @@
       <c r="H90">
         <v>3919.068115</v>
       </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I90" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A91">
         <f>A89+10</f>
         <v>580</v>
@@ -3501,10 +3757,10 @@
         <v>57</v>
       </c>
       <c r="D91" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A92">
         <f>A91+10</f>
         <v>590</v>
@@ -3516,10 +3772,10 @@
         <v>22</v>
       </c>
       <c r="D92" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A93">
         <f>A92+10</f>
         <v>600</v>
@@ -3531,7 +3787,7 @@
         <v>38</v>
       </c>
       <c r="D93" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E93">
         <v>103</v>
@@ -3545,10 +3801,13 @@
       <c r="H93">
         <v>3921.3127439999898</v>
       </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I93" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E94">
         <v>104</v>
@@ -3561,6 +3820,9 @@
       </c>
       <c r="H94">
         <v>3920.9658199999899</v>
+      </c>
+      <c r="I94" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>